<commit_message>
Automation Toolkit Release v10.1
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-CIS-ManagementServices-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-CIS-ManagementServices-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop\cd3_automation_toolkit\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unamachi\Desktop\code\cd3_sch_25022023\oci\cd3_automation_toolkit\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EA394D-794C-401C-A76B-9E304635DD43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DE14B8-A10D-4E4B-B37F-21DDB8672D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2267" uniqueCount="1256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="1269">
   <si>
     <t>Region</t>
   </si>
@@ -4104,13 +4104,40 @@
     <t>Network&amp;prod_vcn</t>
   </si>
   <si>
-    <t>Network&amp;nonprod_vcn</t>
-  </si>
-  <si>
     <t>Network&amp;Audit_In_Subcompartment</t>
   </si>
   <si>
     <t>AppDev&amp;Audit</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Network&amp;nonprod_vcn&amp;nonprod-web</t>
+  </si>
+  <si>
+    <t>Source Monitoring Details</t>
+  </si>
+  <si>
+    <t>Target Monitoring Details</t>
+  </si>
+  <si>
+    <t>Target Function Details</t>
+  </si>
+  <si>
+    <t>monitoring</t>
+  </si>
+  <si>
+    <t>SCH-05</t>
+  </si>
+  <si>
+    <t>logging to monitoring</t>
+  </si>
+  <si>
+    <t>Network&amp;network-vcn-logs&amp;all</t>
+  </si>
+  <si>
+    <t>Network&amp;[CpuUtilization,computeagent]</t>
   </si>
   <si>
     <r>
@@ -4148,7 +4175,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Row 4 below will collect Audit Logs for compartment AppDev and Row 5 will collect Audit Logs for compartment Network and its child compartments.</t>
+      <t xml:space="preserve">Row 4 below will collect Audit Logs for compartment AppDev and Row 5 will collect Audit Logs for compartment Network and its child compartments.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"To enable Source as Log Groups":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Row 6 will collect logs for 'nonprod-web' log under Log Group 'nonprod_vcn' in compartment Network. Row 7 will collect all logs under Log Group 'prod_vcn' in compartment Network.</t>
     </r>
     <r>
       <rPr>
@@ -4170,7 +4219,73 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>is optional field.</t>
+      <t xml:space="preserve">is optional field.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Source Monitoring Details" : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Format is  &lt;compartment_name&gt;&amp;[namespace_name]. Ex: CD3Comp&amp;[oci_blockstorage,oci_computeagent]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Target Monitoring Details" : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Format is &lt;compartment_name&gt;&amp;[metric_name, namespace_name]. For example, check Row 9.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Target Function Details"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Format is &lt;compartment_name&gt;@&lt;application_name&gt;@&lt;function_name&gt;. For example, check Row 10.</t>
     </r>
     <r>
       <rPr>
@@ -4197,6 +4312,40 @@
                              Example: Operations.CostCenter=01;Users.Name=user01
 </t>
     </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CIS LZ recommends to create SCH to collect audit logs for all compartments, VCN Flow Logs and Object Storage Logs and send to a particular target that can be read by SIEM.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>SCH-06</t>
+  </si>
+  <si>
+    <t>stream to function</t>
+  </si>
+  <si>
+    <t>Security@subnet-events@test-func</t>
+  </si>
+  <si>
+    <t>SCH-07</t>
   </si>
 </sst>
 </file>
@@ -4474,7 +4623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4552,6 +4701,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6521,10 +6671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6536,6 +6686,11 @@
     <row r="2" spans="1:1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>1172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1254</v>
       </c>
     </row>
   </sheetData>
@@ -6564,15 +6719,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>1177</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -6824,20 +6979,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>1178</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -9671,22 +9826,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>1179</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="41"/>
     </row>
     <row r="2" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -10118,39 +10273,46 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O648"/>
+  <dimension ref="A1:R649"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="7" max="7" width="18.453125" customWidth="1"/>
-    <col min="8" max="8" width="19.36328125" customWidth="1"/>
-    <col min="15" max="15" width="8.90625" customWidth="1"/>
+    <col min="8" max="9" width="19.36328125" customWidth="1"/>
+    <col min="12" max="12" width="21.26953125" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="31.08984375" customWidth="1"/>
+    <col min="17" max="17" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="125" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-    </row>
-    <row r="2" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="165" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+    </row>
+    <row r="2" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
@@ -10176,28 +10338,37 @@
         <v>1184</v>
       </c>
       <c r="I2" s="27" t="s">
+        <v>1256</v>
+      </c>
+      <c r="J2" s="27" t="s">
         <v>1185</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="K2" s="27" t="s">
         <v>1186</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="L2" s="27" t="s">
         <v>1187</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="M2" s="27" t="s">
         <v>1188</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="N2" s="27" t="s">
         <v>1189</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="O2" s="27" t="s">
         <v>1190</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="P2" s="27" t="s">
+        <v>1257</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>1258</v>
+      </c>
+      <c r="R2" s="29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>1174</v>
       </c>
@@ -10208,15 +10379,18 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
-      <c r="I3" s="8"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="8"/>
-    </row>
-    <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="N3" s="8"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="8"/>
+    </row>
+    <row r="4" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>7</v>
       </c>
@@ -10227,29 +10401,32 @@
         <v>1191</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>1192</v>
+        <v>1197</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>1193</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>1194</v>
+        <v>1198</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="22" t="s">
-        <v>1195</v>
+        <v>1247</v>
       </c>
       <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="22"/>
-    </row>
-    <row r="5" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+    </row>
+    <row r="5" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
@@ -10269,20 +10446,23 @@
         <v>1198</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
-      <c r="K5" s="22" t="s">
+      <c r="K5" s="22"/>
+      <c r="L5" s="22" t="s">
         <v>1247</v>
       </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="30"/>
       <c r="O5" s="22"/>
-    </row>
-    <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+    </row>
+    <row r="6" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>7</v>
       </c>
@@ -10290,32 +10470,35 @@
         <v>574</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>1196</v>
+        <v>1199</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>1197</v>
+        <v>1192</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>1193</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
-      <c r="K6" s="22" t="s">
-        <v>1247</v>
-      </c>
+      <c r="K6" s="22"/>
       <c r="L6" s="22"/>
-      <c r="M6" s="30"/>
+      <c r="M6" s="22" t="s">
+        <v>1195</v>
+      </c>
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
-    </row>
-    <row r="7" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+    </row>
+    <row r="7" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>7</v>
       </c>
@@ -10323,7 +10506,7 @@
         <v>574</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>1199</v>
+        <v>1202</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>1200</v>
@@ -10342,13 +10525,16 @@
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="22" t="s">
+      <c r="M7" s="22"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="22" t="s">
         <v>1248</v>
       </c>
-      <c r="O7" s="22"/>
-    </row>
-    <row r="8" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+    </row>
+    <row r="8" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>7</v>
       </c>
@@ -10356,7 +10542,7 @@
         <v>574</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>1202</v>
+        <v>1260</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>1203</v>
@@ -10371,47 +10557,114 @@
       <c r="H8" s="22" t="s">
         <v>1249</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="22"/>
+      <c r="J8" s="22" t="s">
         <v>1205</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="K8" s="22" t="s">
         <v>1250</v>
       </c>
-      <c r="K8" s="22"/>
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="1:18" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>1259</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>1262</v>
+      </c>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22" t="s">
+        <v>1263</v>
+      </c>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+    </row>
+    <row r="10" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22" t="s">
+        <v>1249</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22" t="s">
+        <v>1267</v>
+      </c>
+      <c r="R10" s="22"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E13" s="31"/>
       <c r="F13" s="31"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E16" s="31"/>
       <c r="F16" s="31"/>
     </row>
@@ -12896,6 +13149,7 @@
       <c r="F636" s="31"/>
     </row>
     <row r="637" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E637" s="31"/>
       <c r="F637" s="31"/>
     </row>
     <row r="638" spans="5:6" x14ac:dyDescent="0.35">
@@ -12931,22 +13185,19 @@
     <row r="648" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F648" s="31"/>
     </row>
+    <row r="649" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F649" s="31"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source_Kind" sqref="E1:E3 E8:E636" xr:uid="{00000000-0002-0000-0400-000000000000}">
-      <formula1>"logging,streaming"</formula1>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{C4DFA3D7-FEF9-4102-B2C1-9A5710644E88}">
+      <formula1>"logging,streaming,monitoring"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Target_Kind" sqref="F1:F3 F5:F648" xr:uid="{00000000-0002-0000-0400-000001000000}">
-      <formula1>"loggingAnalytics,streaming,objectStorage,notifications"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Target_Kind" prompt="Accepted values should be one of them - (loggingAnalytics,streaming,objectStorage,notifications)" sqref="F4" xr:uid="{00000000-0002-0000-0400-000002000000}">
-      <formula1>"loggingAnalytics,streaming,objectStorage,notifications"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Source_Kind" prompt="Source kind should be one of them - (logging,monitoring,streaming)" sqref="E4:E7" xr:uid="{00000000-0002-0000-0400-000003000000}">
-      <formula1>"logging,streaming"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{B4A48907-D395-44AB-8063-4FF2E423056B}">
+      <formula1>"loggingAnalytics,streaming,monitoring,objectStorage,notifications,functions"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Automation Toolkit Release v2024.4.1
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-CIS-ManagementServices-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-CIS-ManagementServices-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/CD3Lasya/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECB66D2-0022-2942-822F-88D89C0065AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CF03FD-3EEF-2345-9220-EDD816DBA032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="760" windowWidth="15840" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="1269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2289" uniqueCount="1279">
   <si>
     <t>Region</t>
   </si>
@@ -4320,10 +4320,36 @@
     <t>deletelocalpeeringgateway.end</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
+    <t>##Commercial##</t>
+  </si>
+  <si>
+    <t>Bogota</t>
+  </si>
+  <si>
+    <t>Jovanovac</t>
+  </si>
+  <si>
+    <t>Monterrey</t>
+  </si>
+  <si>
+    <t>Newport</t>
+  </si>
+  <si>
+    <t>Riyadh</t>
+  </si>
+  <si>
+    <t>Valparaiso</t>
+  </si>
+  <si>
+    <t>##US Gov##</t>
+  </si>
+  <si>
+    <t>##US Defence##</t>
+  </si>
+  <si>
+    <t>##UK Gov##</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -4354,7 +4380,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Release - v2024.4.0</t>
+      <t>Release - v2024.4.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ Updated Region column drop down for all sheets </t>
     </r>
   </si>
 </sst>
@@ -4362,7 +4399,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4423,8 +4460,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4464,6 +4508,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4629,11 +4684,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4726,8 +4782,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -6660,7 +6726,7 @@
     <row r="1" spans="1:1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>1268</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
@@ -6684,7 +6750,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
@@ -6915,9 +6981,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select an OCI Region" xr:uid="{2D820C29-1002-204D-B00D-804EDEB71B8E}">
+        <x14:dataValidation type="list" allowBlank="1" prompt="Select an OCI Region" xr:uid="{2D820C29-1002-204D-B00D-804EDEB71B8E}">
           <x14:formula1>
-            <xm:f>AlarmsTable!$D$2:$D$43</xm:f>
+            <xm:f>AlarmsTable!$D$2:$D$54</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A1048576</xm:sqref>
         </x14:dataValidation>
@@ -9729,9 +9795,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select an OCI Region" xr:uid="{CAEBC965-9C10-D548-BA4C-C9886C31C633}">
+        <x14:dataValidation type="list" allowBlank="1" prompt="Select an OCI Region" xr:uid="{925324F3-2567-D64A-AA03-BB8837367917}">
           <x14:formula1>
-            <xm:f>AlarmsTable!$D$2:$D$43</xm:f>
+            <xm:f>AlarmsTable!$D$2:$D$54</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A1048576</xm:sqref>
         </x14:dataValidation>
@@ -10180,12 +10246,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select an OCI Region" xr:uid="{2F6F6B03-F9DD-654D-A220-710C45591F5F}">
-          <x14:formula1>
-            <xm:f>AlarmsTable!$D$2:$D$43</xm:f>
-          </x14:formula1>
-          <xm:sqref>A3:A1048576</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{3A7701B9-9CDA-494A-8E71-6A5D815A2B37}">
           <x14:formula1>
             <xm:f>AlarmsTable!$A$2:$A$5</xm:f>
@@ -10203,6 +10263,12 @@
             <xm:f>AlarmsTable!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>L3:L1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" prompt="Select an OCI Region" xr:uid="{037041F5-9456-1C44-AC21-3DB92DF323E1}">
+          <x14:formula1>
+            <xm:f>AlarmsTable!$D$2:$D$54</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -13144,9 +13210,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select an OCI Region" xr:uid="{547D9943-C785-B24F-8633-2FB0C1D4FDB0}">
+        <x14:dataValidation type="list" allowBlank="1" prompt="Select an OCI Region" xr:uid="{03D11048-F290-6B43-BA8B-72D4CBD50156}">
           <x14:formula1>
-            <xm:f>AlarmsTable!$D$2:$D$43</xm:f>
+            <xm:f>AlarmsTable!$D$2:$D$54</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A1048576</xm:sqref>
         </x14:dataValidation>
@@ -13160,8 +13226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13196,8 +13262,8 @@
       <c r="C2" s="31" t="s">
         <v>652</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>1233</v>
+      <c r="D2" s="42" t="s">
+        <v>1268</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13211,7 +13277,7 @@
         <v>655</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -13224,8 +13290,8 @@
       <c r="C4" s="31" t="s">
         <v>658</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>1205</v>
+      <c r="D4" t="s">
+        <v>1234</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -13235,48 +13301,48 @@
       <c r="B5" s="7" t="s">
         <v>660</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>1235</v>
+      <c r="D5" t="s">
+        <v>1205</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>661</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>1206</v>
+      <c r="D6" t="s">
+        <v>1269</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>662</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>1207</v>
+      <c r="D7" t="s">
+        <v>1235</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>663</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>1236</v>
+      <c r="D8" t="s">
+        <v>1206</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>1237</v>
+      <c r="D9" t="s">
+        <v>1207</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
         <v>665</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>1228</v>
+      <c r="D10" t="s">
+        <v>1236</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -13284,8 +13350,8 @@
         <v>666</v>
       </c>
       <c r="C11" s="32"/>
-      <c r="D11" s="8" t="s">
-        <v>1232</v>
+      <c r="D11" t="s">
+        <v>1237</v>
       </c>
       <c r="E11" s="33"/>
     </row>
@@ -13293,239 +13359,239 @@
       <c r="B12" s="7" t="s">
         <v>667</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>1229</v>
+      <c r="D12" t="s">
+        <v>1238</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>668</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>1231</v>
+      <c r="D13" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
         <v>669</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>1230</v>
+      <c r="D14" t="s">
+        <v>1209</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
         <v>670</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>1238</v>
+      <c r="D15" t="s">
+        <v>1210</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>1208</v>
+      <c r="D16" t="s">
+        <v>1270</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
         <v>672</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>1209</v>
+      <c r="D17" t="s">
+        <v>1211</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
         <v>673</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>1210</v>
+      <c r="D18" t="s">
+        <v>1212</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>674</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>1239</v>
+      <c r="D19" t="s">
+        <v>1213</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>1211</v>
+      <c r="D20" t="s">
+        <v>1214</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>676</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>1240</v>
+      <c r="D21" t="s">
+        <v>1215</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>677</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>1212</v>
+      <c r="D22" t="s">
+        <v>1216</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>678</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>1213</v>
+      <c r="D23" t="s">
+        <v>1271</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>679</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>1214</v>
+      <c r="D24" t="s">
+        <v>1241</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>1215</v>
+      <c r="D25" t="s">
+        <v>1272</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
         <v>681</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>1216</v>
+      <c r="D26" t="s">
+        <v>1217</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
         <v>682</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>1241</v>
+      <c r="D27" t="s">
+        <v>1242</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="7" t="s">
         <v>683</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>1217</v>
+      <c r="D28" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>1242</v>
+      <c r="D29" t="s">
+        <v>1218</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="7" t="s">
         <v>685</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>7</v>
+      <c r="D30" t="s">
+        <v>1273</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="7" t="s">
         <v>686</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>1218</v>
+      <c r="D31" t="s">
+        <v>1219</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="7" t="s">
         <v>687</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>1219</v>
+      <c r="D32" t="s">
+        <v>1220</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>1220</v>
+      <c r="D33" t="s">
+        <v>1243</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>688</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>1243</v>
+      <c r="D34" t="s">
+        <v>1221</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>689</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>1221</v>
+      <c r="D35" t="s">
+        <v>1222</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>690</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>1222</v>
+      <c r="D36" t="s">
+        <v>1244</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>691</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>1244</v>
+      <c r="D37" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>692</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>1223</v>
+      <c r="D38" t="s">
+        <v>1224</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="7" t="s">
         <v>693</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>1224</v>
+      <c r="D39" t="s">
+        <v>1225</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" s="7" t="s">
         <v>694</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>1225</v>
+      <c r="D40" s="43" t="s">
+        <v>1274</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="7" t="s">
         <v>695</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" t="s">
         <v>1226</v>
       </c>
     </row>
@@ -13533,71 +13599,104 @@
       <c r="B42" s="7" t="s">
         <v>696</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>1227</v>
+      <c r="D42" t="s">
+        <v>1218</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="7" t="s">
         <v>697</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>1172</v>
+      <c r="D43" t="s">
+        <v>1227</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="7" t="s">
         <v>698</v>
       </c>
+      <c r="D44" s="44" t="s">
+        <v>1275</v>
+      </c>
     </row>
     <row r="45" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="7" t="s">
         <v>699</v>
       </c>
+      <c r="D45" t="s">
+        <v>1239</v>
+      </c>
     </row>
     <row r="46" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="7" t="s">
         <v>700</v>
       </c>
+      <c r="D46" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="47" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="7" t="s">
         <v>701</v>
       </c>
+      <c r="D47" s="5" t="s">
+        <v>1276</v>
+      </c>
     </row>
     <row r="48" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="7" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="7" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="D51" s="5" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="7" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="7" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" s="7" t="s">
         <v>708</v>
+      </c>
+      <c r="D54" s="43" t="s">
+        <v>1172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CD3 Automation Toolkit Release v2025.2.0
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-CIS-ManagementServices-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-CIS-ManagementServices-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop1/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD136FD5-49B4-3D48-8C63-4712A74A4B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9A8B70-5702-6A48-9F42-DA0101531AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1920" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -4347,6 +4347,12 @@
     </r>
   </si>
   <si>
+    <t>Singapore-1</t>
+  </si>
+  <si>
+    <t>Singapore-2</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -4377,7 +4383,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Release - v2024.4.3</t>
+      <t xml:space="preserve">Release - v2025.2.0
+</t>
     </r>
     <r>
       <rPr>
@@ -4387,15 +4394,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
- Modified description in KMS sheet, Modified delimiters in ServiceConectors sheet</t>
+      <t xml:space="preserve">Modified Notifications backend code
+</t>
     </r>
-  </si>
-  <si>
-    <t>Singapore-1</t>
-  </si>
-  <si>
-    <t>Singapore-2</t>
   </si>
 </sst>
 </file>
@@ -6718,7 +6719,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6729,7 +6730,7 @@
     <row r="1" spans="1:1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>1277</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
@@ -13548,12 +13549,12 @@
         <v>689</v>
       </c>
       <c r="D35" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="16" x14ac:dyDescent="0.2">

</xml_diff>